<commit_message>
Make the test pass till 2022
</commit_message>
<xml_diff>
--- a/src/test/resources/database-site.xlsx
+++ b/src/test/resources/database-site.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15615" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15615" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Speakers" sheetId="1" r:id="rId1"/>
@@ -5789,7 +5789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -5999,7 +5999,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6067,11 +6069,11 @@
         <v>40849</v>
       </c>
       <c r="F2" s="19">
-        <v>42673</v>
+        <v>44499</v>
       </c>
       <c r="G2" s="21">
         <f>F2+DATE(D2/5,1,-1)</f>
-        <v>43038</v>
+        <v>44864</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>57</v>
@@ -6084,7 +6086,7 @@
       </c>
       <c r="K2" s="23">
         <f ca="1">IF(G2&gt;NOW(),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>

</xml_diff>

<commit_message>
Correction donnees test afin que les tests soient passants
</commit_message>
<xml_diff>
--- a/src/test/resources/database-site.xlsx
+++ b/src/test/resources/database-site.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Speakers" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -83,85 +83,88 @@
     <t xml:space="preserve">logoUrl</t>
   </si>
   <si>
+    <t xml:space="preserve">targetUrl</t>
+  </si>
+  <si>
     <t xml:space="preserve">endOfValidity</t>
   </si>
   <si>
+    <t xml:space="preserve">DEVCOOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.devcoop.fr/img/logo.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.devcoop.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31/12/2050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lh3.googleusercontent.com/r4YEXflD_fJMBDWRLI2o7diZxM4XpcCOeQzSxRh58XaTepZpl8GUT1Ae1FJ7PutZlc1ma1Dr_YdM=w158-h60-no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://global.agfahealthcare.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31/12/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPPON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.ipponusa.com/wp-content/uploads/2014/03/logo_Ippontech14011.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.ippon.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUDENSIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audensiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.audensiel.com/templates/gkn/img/logo_gkn.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.audensiel.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CleverCloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.clever-cloud.com/images/icons/logo.svg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.clever-cloud.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31/12/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speakerID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cospeakerID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">summary</t>
+  </si>
+  <si>
     <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEVCOOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.devcoop.fr/img/logo.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.devcoop.fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31/12/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGFA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://lh3.googleusercontent.com/r4YEXflD_fJMBDWRLI2o7diZxM4XpcCOeQzSxRh58XaTepZpl8GUT1Ae1FJ7PutZlc1ma1Dr_YdM=w158-h60-no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://global.agfahealthcare.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31/12/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPPON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.ipponusa.com/wp-content/uploads/2014/03/logo_Ippontech14011.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.ippon.fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUDENSIEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audensiel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.audensiel.com/templates/gkn/img/logo_gkn.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.audensiel.fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CleverCloud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.clever-cloud.com/images/icons/logo.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.clever-cloud.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31/12/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">speakerID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cospeakerID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locationID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">summary</t>
   </si>
   <si>
     <t xml:space="preserve">eventMeetupId</t>
@@ -271,11 +274,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00&quot; €&quot;"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00&quot; €&quot;"/>
+    <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -420,7 +424,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,23 +457,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -481,23 +497,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,13 +527,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -583,22 +599,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="45.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="121.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,10 +686,10 @@
       <c r="C3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
@@ -1678,6 +1692,9 @@
     <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:E3"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://sites.google.com/site/jugsummercamp/_/rsrc/1308231479541/edition2010/speakers/julienDubois.jpg"/>
   </hyperlinks>
@@ -1692,22 +1709,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1720,10 +1736,10 @@
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F1" s="3"/>
@@ -1749,89 +1765,96 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1854,7 +1877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1864,11 +1887,9 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="145.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1890,17 +1911,17 @@
       <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="H1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="I1" s="14" t="s">
         <v>47</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -1924,7 +1945,7 @@
       <c r="A2" s="4" t="n">
         <v>20141204</v>
       </c>
-      <c r="B2" s="12" t="n">
+      <c r="B2" s="15" t="n">
         <v>41977</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1934,16 +1955,16 @@
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1958,7 +1979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1968,41 +1989,38 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="I1" s="16" t="s">
         <v>61</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -2022,39 +2040,39 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="16" t="n">
+        <v>65</v>
+      </c>
+      <c r="D2" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="E2" s="17" t="n">
+      <c r="E2" s="20" t="n">
         <v>40849</v>
       </c>
-      <c r="F2" s="17" t="n">
+      <c r="F2" s="20" t="n">
         <v>44499</v>
       </c>
-      <c r="G2" s="18" t="n">
+      <c r="G2" s="21" t="n">
         <f aca="false">F2+DATE(D2/5,1,-1)</f>
         <v>44864</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" s="19" t="n">
+        <v>68</v>
+      </c>
+      <c r="K2" s="22" t="n">
         <f aca="true">IF(G2&gt;NOW(),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -2083,7 +2101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2093,11 +2111,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2108,19 +2124,19 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="14" t="s">
         <v>72</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -2144,22 +2160,22 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="20" t="s">
         <v>74</v>
       </c>
+      <c r="C2" s="23" t="s">
+        <v>75</v>
+      </c>
       <c r="D2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="21" t="s">
         <v>76</v>
       </c>
+      <c r="E2" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="F2" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>10903542</v>

</xml_diff>